<commit_message>
Fixing senesced leaf model
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Soybean/Observed.xlsx
+++ b/Tests/UnderReview/Soybean/Observed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Soybean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\UnderReview\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1148BF-0AA3-424A-B401-BDE2B7AB794E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487AEFBF-F542-4F0A-AD59-03029F120FBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="338">
   <si>
     <t>SimulationName</t>
   </si>
@@ -1047,6 +1047,9 @@
   </si>
   <si>
     <t>SoilNH4_30cm</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.CoverTotal</t>
   </si>
 </sst>
 </file>
@@ -3995,11 +3998,11 @@
   <dimension ref="A1:CR336"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10716" ySplit="576" topLeftCell="Q250" activePane="bottomLeft"/>
+      <pane xSplit="10716" ySplit="576" topLeftCell="O1" activePane="bottomRight"/>
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="topRight" activeCell="R1" sqref="R1:R1048576"/>
       <selection pane="bottomLeft" activeCell="C341" sqref="C341"/>
-      <selection pane="bottomRight" activeCell="Q225" sqref="Q225"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4133,7 +4136,7 @@
         <v>55</v>
       </c>
       <c r="O1" t="s">
-        <v>182</v>
+        <v>337</v>
       </c>
       <c r="P1" t="s">
         <v>91</v>

</xml_diff>